<commit_message>
MAJ Poster RDV MEL
</commit_message>
<xml_diff>
--- a/Suivi_de_projet/graph.xlsx
+++ b/Suivi_de_projet/graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avere\Documents\Cours\Projet PPAL\Projet PPAL\Suivi_de_projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxou\Documents\4ème année ISEN\Prédiction pollution air Lille\Projet-AirIQ\Suivi_de_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29F3B80B-07E5-48B3-B504-2A75C378A7E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECD5614-60D0-40AD-8157-3E9D5FF5AD0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graph" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -591,7 +591,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -604,14 +604,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="fr-FR" sz="1800"/>
+              <a:rPr lang="fr-FR" sz="2400"/>
               <a:t>Prédiction</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="fr-FR" sz="1800" baseline="0"/>
+              <a:rPr lang="fr-FR" sz="2400" baseline="0"/>
               <a:t> de la qualité de l'air par notre modèle</a:t>
             </a:r>
-            <a:endParaRPr lang="fr-FR" sz="1800"/>
+            <a:endParaRPr lang="fr-FR" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -628,7 +628,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1918,7 +1918,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1931,7 +1931,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Jours</a:t>
                 </a:r>
               </a:p>
@@ -1950,7 +1950,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2004,7 +2004,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2017,7 +2017,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Indice de qualité de l'air</a:t>
                 </a:r>
               </a:p>
@@ -2036,7 +2036,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2097,6 +2097,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.43869674267804354"/>
+          <c:y val="0.1230417760279965"/>
+          <c:w val="0.15548522255030617"/>
+          <c:h val="6.3663823272090983E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2110,7 +2120,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2731,15 +2741,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>79374</xdr:colOff>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2771,23 +2781,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>114594</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>120539</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>165861</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>172340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="4" name="Image 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E2024FD-C308-49F4-9FAE-D4D76FBE465A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA10CF9-8DBB-413E-BB56-0250A89B5104}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2803,8 +2813,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="241300" y="139700"/>
-          <a:ext cx="15113294" cy="4584589"/>
+          <a:off x="3048000" y="736600"/>
+          <a:ext cx="14643861" cy="4407790"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3112,10 +3122,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -4680,11 +4690,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>